<commit_message>
Make glossary table header sticky
</commit_message>
<xml_diff>
--- a/Data/TrustMark_Glossary raw file.xlsx
+++ b/Data/TrustMark_Glossary raw file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Glossary WIP\trustmark-glossary\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2B801E-57F6-4760-88C9-751CE67C58D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221A434A-5DD4-4033-BD9D-931C40F9B633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="18408" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1004,14 +1004,6 @@
     <t>RSS = 100 x (((6 x sum Cat1 measures) + (3 x sum Major measures) + sum Minor measures)/sum measures audited)/6</t>
   </si>
   <si>
-    <t>The construct of the metric assigns a different weight to the severity of the non-compliance as follows;
-Cat1: 6
-Major: 3
-Minor: 1
-So, a Cat1 non compliance is considered to be twice as severe as a Major and 6 times more severe than a Minor non compliance. These weights have been defined deterministically and can be altered if required in future development work. Essentially this produces a weighted average of the severity of the non compliance across the measures in a project, or any level of aggregation such as an individual installer, RC, RA etc.
-The score is thenm normalised to a range of 0 to 100 by initially dividing by 6. If all the measures were a Cat1 then the total score would be 6, so dividing by 6 brings it in the range of 0 to 1. For easier use, the score is then multiplied by 100 to convert into a range from 0 to 100.</t>
-  </si>
-  <si>
     <t>DoC</t>
   </si>
   <si>
@@ -2474,6 +2466,15 @@
   </si>
   <si>
     <t>Website Analytics Reports</t>
+  </si>
+  <si>
+    <t>"Risk Severity Score"
+The construct of the metric assigns a different weight to the severity of the non-compliance as follows;
+Cat1: 6
+Major: 3
+Minor: 1
+So, a Cat1 non compliance is considered to be twice as severe as a Major and 6 times more severe than a Minor non compliance. These weights have been defined deterministically and can be altered if required in future development work. Essentially this produces a weighted average of the severity of the non compliance across the measures in a project, or any level of aggregation such as an individual installer, RC, RA etc.
+The score is then normalised to a range of 0 to 100 by initially dividing by 6. If all the measures were a Cat1 then the total score would be 6, so dividing by 6 brings it in the range of 0 to 1. For easier use, the score is then multiplied by 100 to convert into a range from 0 to 100.</t>
   </si>
 </sst>
 </file>
@@ -2942,8 +2943,8 @@
   <dimension ref="A1:F235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2979,10 +2980,10 @@
     </row>
     <row r="2" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
@@ -2991,15 +2992,15 @@
         <v>312</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>26</v>
@@ -3008,18 +3009,18 @@
         <v>312</v>
       </c>
       <c r="E3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>26</v>
@@ -3028,18 +3029,18 @@
         <v>312</v>
       </c>
       <c r="E4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>26</v>
@@ -3048,15 +3049,15 @@
         <v>312</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>26</v>
@@ -3065,18 +3066,18 @@
         <v>312</v>
       </c>
       <c r="E6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -3085,15 +3086,15 @@
         <v>312</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>26</v>
@@ -3102,18 +3103,18 @@
         <v>312</v>
       </c>
       <c r="E8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>26</v>
@@ -3122,15 +3123,15 @@
         <v>312</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>26</v>
@@ -3139,15 +3140,15 @@
         <v>312</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>26</v>
@@ -3156,15 +3157,15 @@
         <v>312</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>26</v>
@@ -3173,18 +3174,18 @@
         <v>312</v>
       </c>
       <c r="E12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
@@ -3193,15 +3194,15 @@
         <v>312</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="114.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>26</v>
@@ -3210,15 +3211,15 @@
         <v>312</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>26</v>
@@ -3227,15 +3228,15 @@
         <v>312</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>26</v>
@@ -3244,15 +3245,15 @@
         <v>312</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>26</v>
@@ -3261,15 +3262,15 @@
         <v>312</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>26</v>
@@ -3278,18 +3279,18 @@
         <v>312</v>
       </c>
       <c r="E18" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>23</v>
@@ -3298,15 +3299,15 @@
         <v>312</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>26</v>
@@ -3315,15 +3316,15 @@
         <v>312</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
@@ -3332,15 +3333,15 @@
         <v>312</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>26</v>
@@ -3349,18 +3350,18 @@
         <v>312</v>
       </c>
       <c r="E22" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
@@ -3369,18 +3370,18 @@
         <v>312</v>
       </c>
       <c r="E23" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>26</v>
@@ -3389,15 +3390,15 @@
         <v>312</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>26</v>
@@ -3406,15 +3407,15 @@
         <v>312</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>511</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>512</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>23</v>
@@ -3423,10 +3424,10 @@
         <v>314</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
@@ -3443,12 +3444,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>485</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>7</v>
@@ -3457,12 +3458,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>7</v>
@@ -3471,7 +3472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -3488,7 +3489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
@@ -3505,7 +3506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
@@ -3522,15 +3523,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>18</v>
       </c>
@@ -3547,12 +3548,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>494</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>26</v>
@@ -3561,26 +3562,26 @@
         <v>313</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>509</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>23</v>
@@ -3589,10 +3590,10 @@
         <v>314</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -3610,7 +3611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
@@ -3627,7 +3628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>27</v>
       </c>
@@ -3647,12 +3648,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>491</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>23</v>
@@ -3661,15 +3662,15 @@
         <v>313</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>23</v>
@@ -3678,7 +3679,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>315</v>
       </c>
@@ -3715,15 +3716,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>32</v>
       </c>
@@ -3757,7 +3758,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>37</v>
       </c>
@@ -3774,12 +3775,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>526</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>527</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>26</v>
@@ -3788,10 +3789,10 @@
         <v>313</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3828,7 +3829,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>44</v>
       </c>
@@ -3847,18 +3848,18 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>7</v>
@@ -3901,7 +3902,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>52</v>
       </c>
@@ -3918,7 +3919,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>54</v>
       </c>
@@ -3952,7 +3953,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
@@ -3969,7 +3970,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
@@ -3986,12 +3987,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>505</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>506</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>23</v>
@@ -4000,10 +4001,10 @@
         <v>313</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
@@ -4022,10 +4023,10 @@
     </row>
     <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>529</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>530</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>26</v>
@@ -4034,13 +4035,13 @@
         <v>313</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
@@ -4057,7 +4058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -4074,7 +4075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
@@ -4091,12 +4092,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -4117,7 +4118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>73</v>
       </c>
@@ -4151,12 +4152,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>479</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>7</v>
@@ -4165,12 +4166,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4190,7 +4191,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>79</v>
       </c>
@@ -4208,20 +4209,20 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>322</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>7</v>
@@ -4230,7 +4231,7 @@
         <v>310</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4250,12 +4251,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>7</v>
@@ -4282,7 +4283,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>85</v>
       </c>
@@ -4299,15 +4300,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>87</v>
       </c>
@@ -4324,12 +4325,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>489</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>7</v>
@@ -4355,12 +4356,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>23</v>
@@ -4374,7 +4375,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>95</v>
@@ -4391,7 +4392,7 @@
     </row>
     <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>96</v>
@@ -4408,10 +4409,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4434,12 +4435,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>26</v>
@@ -4448,21 +4449,21 @@
         <v>313</v>
       </c>
       <c r="E91" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="F91" s="2" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>97</v>
       </c>
@@ -4479,7 +4480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>100</v>
       </c>
@@ -4498,10 +4499,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>417</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>7</v>
@@ -4510,7 +4511,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>102</v>
       </c>
@@ -4546,13 +4547,13 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>106</v>
       </c>
@@ -4569,7 +4570,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>108</v>
       </c>
@@ -4589,7 +4590,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>111</v>
       </c>
@@ -4606,28 +4607,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>514</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>515</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>23</v>
@@ -4636,15 +4637,15 @@
         <v>314</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4698,23 +4699,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>120</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>127</v>
       </c>
@@ -4785,7 +4786,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>129</v>
       </c>
@@ -4803,7 +4804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>131</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>133</v>
       </c>
@@ -4837,7 +4838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>135</v>
       </c>
@@ -4872,12 +4873,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>7</v>
@@ -4886,7 +4887,7 @@
         <v>312</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4908,10 +4909,10 @@
     </row>
     <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>502</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>26</v>
@@ -4920,18 +4921,18 @@
         <v>313</v>
       </c>
       <c r="E122" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>520</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>521</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>23</v>
@@ -4940,7 +4941,7 @@
         <v>314</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4960,7 +4961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>143</v>
       </c>
@@ -4977,7 +4978,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>145</v>
       </c>
@@ -4994,7 +4995,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>147</v>
       </c>
@@ -5014,7 +5015,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>150</v>
       </c>
@@ -5051,7 +5052,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>155</v>
       </c>
@@ -5068,7 +5069,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>157</v>
       </c>
@@ -5085,7 +5086,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>159</v>
       </c>
@@ -5102,7 +5103,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>161</v>
       </c>
@@ -5137,7 +5138,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>165</v>
       </c>
@@ -5154,7 +5155,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>167</v>
       </c>
@@ -5172,12 +5173,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -5197,15 +5198,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>171</v>
       </c>
@@ -5222,12 +5223,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>415</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>7</v>
@@ -5236,13 +5237,13 @@
         <v>310</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="C142" s="2" t="s">
         <v>23</v>
       </c>
@@ -5250,7 +5251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>173</v>
       </c>
@@ -5267,12 +5268,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>23</v>
@@ -5281,12 +5282,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>23</v>
@@ -5295,7 +5296,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>175</v>
       </c>
@@ -5317,16 +5318,16 @@
         <v>175</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B148" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="C148" s="2" t="s">
         <v>23</v>
       </c>
@@ -5334,7 +5335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>177</v>
       </c>
@@ -5351,7 +5352,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>179</v>
       </c>
@@ -5368,12 +5369,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>23</v>
@@ -5382,12 +5383,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>23</v>
@@ -5413,7 +5414,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>184</v>
       </c>
@@ -5447,7 +5448,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>188</v>
       </c>
@@ -5467,7 +5468,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>191</v>
       </c>
@@ -5484,12 +5485,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>422</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>7</v>
@@ -5498,15 +5499,15 @@
         <v>312</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>193</v>
       </c>
@@ -5523,7 +5524,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>195</v>
       </c>
@@ -5540,12 +5541,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>487</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>7</v>
@@ -5554,7 +5555,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>197</v>
       </c>
@@ -5592,7 +5593,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>202</v>
       </c>
@@ -5610,7 +5611,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>202</v>
       </c>
@@ -5645,12 +5646,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5704,7 +5705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>213</v>
       </c>
@@ -5721,7 +5722,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>215</v>
       </c>
@@ -5738,7 +5739,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>217</v>
       </c>
@@ -5772,7 +5773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>221</v>
       </c>
@@ -5791,10 +5792,10 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>7</v>
@@ -5806,9 +5807,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>223</v>
@@ -5825,10 +5826,10 @@
     </row>
     <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>523</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>524</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>26</v>
@@ -5837,13 +5838,13 @@
         <v>313</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>224</v>
       </c>
@@ -5860,7 +5861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>226</v>
       </c>
@@ -5897,7 +5898,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>231</v>
       </c>
@@ -5914,7 +5915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>233</v>
       </c>
@@ -5966,7 +5967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>239</v>
       </c>
@@ -6003,15 +6004,15 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>233</v>
@@ -6025,13 +6026,13 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>243</v>
       </c>
@@ -6048,12 +6049,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>245</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>320</v>
+        <v>535</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>26</v>
@@ -6068,12 +6069,12 @@
         <v>317</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>7</v>
@@ -6082,7 +6083,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>246</v>
       </c>
@@ -6099,26 +6100,26 @@
         <v>115</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -6138,12 +6139,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -6214,7 +6215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>258</v>
       </c>
@@ -6233,10 +6234,10 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>7</v>
@@ -6279,7 +6280,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>264</v>
       </c>
@@ -6316,7 +6317,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>269</v>
       </c>
@@ -6333,7 +6334,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>271</v>
       </c>
@@ -6350,7 +6351,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>273</v>
       </c>
@@ -6367,7 +6368,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>275</v>
       </c>
@@ -6401,7 +6402,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>279</v>
       </c>
@@ -6436,7 +6437,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>283</v>
       </c>
@@ -6473,7 +6474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>288</v>
       </c>
@@ -6490,7 +6491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>290</v>
       </c>
@@ -6542,12 +6543,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>7</v>
@@ -6556,28 +6557,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>328</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>7</v>
@@ -6639,10 +6640,10 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B230" s="2" t="s">
         <v>517</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>518</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>26</v>
@@ -6651,13 +6652,13 @@
         <v>314</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F230" s="2" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>302</v>
       </c>
@@ -6674,7 +6675,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>304</v>
       </c>
@@ -6691,12 +6692,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="B233" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>533</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>26</v>
@@ -6705,13 +6706,13 @@
         <v>313</v>
       </c>
       <c r="E233" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="F233" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="F233" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>306</v>
       </c>
@@ -6843,6 +6844,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88ebd88c-02b9-4f51-b0de-dd3becf8de8a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="96a83f3b-8347-4ba1-82f9-fe673303b220" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B762B6222AFFCC489B42E0529EE4ABC8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b32ab374fe5bd1b4f05e15c1f64274aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="88ebd88c-02b9-4f51-b0de-dd3becf8de8a" xmlns:ns3="96a83f3b-8347-4ba1-82f9-fe673303b220" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbbfdcc4e129130c2a3db4ea288b45f9" ns2:_="" ns3:_="">
     <xsd:import namespace="88ebd88c-02b9-4f51-b0de-dd3becf8de8a"/>
@@ -7037,17 +7049,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88ebd88c-02b9-4f51-b0de-dd3becf8de8a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="96a83f3b-8347-4ba1-82f9-fe673303b220" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27B72F3A-D025-4AC7-B6CD-F802C9C57606}">
   <ds:schemaRefs>
@@ -7057,6 +7058,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD79C434-4B1B-4646-B50D-548016E545B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="88ebd88c-02b9-4f51-b0de-dd3becf8de8a"/>
+    <ds:schemaRef ds:uri="96a83f3b-8347-4ba1-82f9-fe673303b220"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A3845F5-1D68-48F6-B78B-A45ABA09BE24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7075,17 +7087,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD79C434-4B1B-4646-B50D-548016E545B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="88ebd88c-02b9-4f51-b0de-dd3becf8de8a"/>
-    <ds:schemaRef ds:uri="96a83f3b-8347-4ba1-82f9-fe673303b220"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{c427a8d0-e03b-4e31-b103-627eb3fdd31c}" enabled="0" method="" siteId="{c427a8d0-e03b-4e31-b103-627eb3fdd31c}" removed="1"/>

</xml_diff>